<commit_message>
Minor Updates to remaining hours
</commit_message>
<xml_diff>
--- a/Sprint 1 Backlog.xlsx
+++ b/Sprint 1 Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="36" windowWidth="11460" windowHeight="7944"/>
@@ -123,8 +123,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,6 +293,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,36 +330,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -338,6 +338,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -416,6 +421,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -450,6 +456,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,15 +632,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="51.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -644,31 +651,31 @@
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="21">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="15" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="K2" s="12" t="s">
         <v>20</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -687,45 +694,45 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -738,7 +745,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -748,7 +755,7 @@
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="1">
@@ -757,8 +764,17 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -768,7 +784,7 @@
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="1">
@@ -777,8 +793,17 @@
       <c r="F7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -788,7 +813,7 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1">
@@ -797,8 +822,17 @@
       <c r="F8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -808,7 +842,7 @@
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="1">
@@ -817,8 +851,17 @@
       <c r="F9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -828,7 +871,7 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1">
@@ -837,8 +880,17 @@
       <c r="F10" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -851,7 +903,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -864,11 +916,23 @@
       <c r="D13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
       <c r="F13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>31</v>
       </c>
@@ -881,22 +945,46 @@
       <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
       <c r="F15" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -909,11 +997,23 @@
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
       <c r="F16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -923,7 +1023,19 @@
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
       <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
         <v>0</v>
       </c>
     </row>
@@ -948,20 +1060,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -969,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -977,7 +1089,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -985,7 +1097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -993,17 +1105,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1014,12 +1126,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>